<commit_message>
Revert "v0.2.1 (#36)" (#37)
This reverts commit 7f68e3cb88798b888642b8a7a9d9712f3bdf50c2.
</commit_message>
<xml_diff>
--- a/test/示例表格.xlsx
+++ b/test/示例表格.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Excel2RpyScript\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D04F607-950C-4493-91EE-A5D4E59C785A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEE44AB-3DFD-4E86-A28E-6A9E9C139C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>角色</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -250,22 +249,6 @@
   </si>
   <si>
     <t>haruhi 1 hide</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>"只是不小心被石头绊了一下，\想不%到竟"然"差点'摔'了{下[去。"</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>音效</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>test</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>test sustain</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -719,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -736,7 +719,7 @@
     <col min="28" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -758,7 +741,7 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -778,7 +761,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -798,7 +781,7 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -820,7 +803,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -840,7 +823,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -886,11 +869,8 @@
       <c r="AA6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AB6" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -918,7 +898,7 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
     </row>
-    <row r="8" spans="1:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -957,7 +937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
         <v>16</v>
@@ -980,11 +960,8 @@
       <c r="R9" s="4"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-      <c r="AB9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
@@ -1011,7 +988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
@@ -1035,7 +1012,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:28" ht="40.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="40.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
         <v>19</v>
@@ -1059,7 +1036,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
         <v>20</v>
@@ -1090,7 +1067,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
         <v>21</v>
@@ -1121,7 +1098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
         <v>22</v>
@@ -1144,7 +1121,7 @@
       <c r="R15" s="4"/>
       <c r="S15" s="3"/>
     </row>
-    <row r="16" spans="1:28" ht="34.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="34.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
         <v>23</v>
@@ -1167,9 +1144,6 @@
       <c r="R16" s="4"/>
       <c r="S16" s="3">
         <v>20</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1568,1020 +1542,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1E585A-3D72-480A-9FC9-E529E4853477}">
-  <dimension ref="A1:AA30"/>
-  <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-    </row>
-    <row r="8" spans="1:27" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA8" s="1"/>
-    </row>
-    <row r="9" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-    </row>
-    <row r="10" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-    </row>
-    <row r="11" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-    </row>
-    <row r="12" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-    </row>
-    <row r="13" spans="1:27" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-    </row>
-    <row r="14" spans="1:27" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA14" s="1"/>
-    </row>
-    <row r="15" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-    </row>
-    <row r="16" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="3">
-        <v>20</v>
-      </c>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-    </row>
-    <row r="18" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-    </row>
-    <row r="19" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-    </row>
-    <row r="20" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-    </row>
-    <row r="21" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-    </row>
-    <row r="22" spans="1:27" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-    </row>
-    <row r="23" spans="1:27" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-    </row>
-    <row r="24" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-    </row>
-    <row r="25" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA25" s="1"/>
-    </row>
-    <row r="26" spans="1:27" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="3">
-        <v>22</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA26" s="1"/>
-    </row>
-    <row r="27" spans="1:27" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-    </row>
-    <row r="28" spans="1:27" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-    </row>
-    <row r="29" spans="1:27" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-    </row>
-    <row r="30" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B9:R9"/>
-    <mergeCell ref="A1:R3"/>
-    <mergeCell ref="A4:R6"/>
-    <mergeCell ref="B7:R7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="B8:R8"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B10:R10"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="B13:R13"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B15:R15"/>
-    <mergeCell ref="B16:R16"/>
-    <mergeCell ref="B17:R17"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B19:R19"/>
-    <mergeCell ref="B20:R20"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B25:R25"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="B27:R27"/>
-  </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>